<commit_message>
add file upload api
</commit_message>
<xml_diff>
--- a/Document/BingqiangZhou/document/工作日志.xlsx
+++ b/Document/BingqiangZhou/document/工作日志.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF36772C-0A3A-4288-889D-E8121D871D7C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F23FCE22-5625-48D6-B8F6-E403EA1A0D38}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>时间</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -41,20 +41,20 @@
 三、完善用户管理</t>
   </si>
   <si>
+    <t>一、测试用户管理模块并完善api文档
+二、完善原型设计图
+三、完善系统分析书与需求分析书</t>
+  </si>
+  <si>
+    <t>一、测试用户管理模块并完善api文档
+二、完善原型设计图(完成)
+三、完善系统分析书与需求分析书</t>
+  </si>
+  <si>
     <r>
       <t>一、上传文件（完成）
 二、在线测试模块（完成）
-三、完善用户管理（已完成，</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>待测试</t>
+三、完善用户管理（已完成</t>
     </r>
     <r>
       <rPr>
@@ -68,16 +68,23 @@
     </r>
   </si>
   <si>
-    <t>一、测试用户管理模块并完善api文档
-二、完善原型设计图
-三、完善系统分析书与需求分析书</t>
+    <t>一、重建工程
+二、加入Help Page
+三、加入Test API 组件</t>
+  </si>
+  <si>
+    <t>一、完成后台API</t>
+  </si>
+  <si>
+    <t>一、完成后台API
+二、搜集测试数据</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,13 +97,6 @@
       <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -126,7 +126,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -138,6 +138,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -476,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -516,10 +520,10 @@
         <v>43403</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="45">
@@ -528,6 +532,30 @@
       </c>
       <c r="B4" s="4" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="45">
+      <c r="A5" s="5">
+        <v>43405</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="6">
+        <v>43406</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="30">
+      <c r="A7" s="6">
+        <v>43407</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>